<commit_message>
Flat: latest data (2021-05-20T07:09:06.061Z) {   "date": "2021-05-20T07:09:06.061Z",   "files": [     {       "name": "IRYO-vaccination_data.csv",       "deltaBytes": 50,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data.xlsx"     },     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 37,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t> 内１回目</t>
   </si>
@@ -254,7 +254,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（5月18日時点）</t>
+    <t>（5月19日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -699,7 +699,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -747,537 +747,557 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="6">
-        <f t="shared" ref="C4:C25" si="0">SUM(D4:E4)</f>
-        <v>5730967</v>
+        <f t="shared" ref="C4:C26" si="0">SUM(D4:E4)</f>
+        <v>5998833</v>
       </c>
       <c r="D4" s="6">
-        <v>3695908</v>
+        <v>3784071</v>
       </c>
       <c r="E4" s="6">
-        <v>2035059</v>
+        <v>2214762</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="13">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D5" s="6">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E5" s="6">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="13">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D6" s="6">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E6" s="6">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="13">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D7" s="6">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E7" s="6">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="13">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D8" s="6">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E8" s="6">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="13">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D9" s="6">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E9" s="6">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="13">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D10" s="6">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E10" s="6">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="13">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D11" s="6">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E11" s="6">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="13">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D12" s="6">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E12" s="6">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="13">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D13" s="6">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E13" s="6">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="13">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D14" s="6">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E14" s="6">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="13">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D15" s="6">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E15" s="6">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="13">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D16" s="6">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E16" s="6">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="13">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" s="6">
         <f t="shared" si="0"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D17" s="6">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E17" s="6">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="13">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D18" s="6">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E18" s="6">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="13">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" s="6">
         <f t="shared" si="0"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D19" s="6">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E19" s="6">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="13">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D20" s="6">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E20" s="6">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="13">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D21" s="6">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E21" s="6">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A22" s="15">
-        <v>44305</v>
-      </c>
-      <c r="B22" s="12" t="str">
-        <f t="shared" ref="B22:B25" si="1">"("&amp;TEXT(A22,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A22" s="13">
+        <v>44306</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D22" s="6">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E22" s="6">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A23" s="13">
+      <c r="A23" s="15">
+        <v>44305</v>
+      </c>
+      <c r="B23" s="12" t="str">
+        <f t="shared" ref="B23:B26" si="1">"("&amp;TEXT(A23,"aaa")&amp;")"</f>
+        <v>(月)</v>
+      </c>
+      <c r="C23" s="6">
+        <f t="shared" si="0"/>
+        <v>119032</v>
+      </c>
+      <c r="D23" s="6">
+        <v>64725</v>
+      </c>
+      <c r="E23" s="6">
+        <v>54307</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A24" s="13">
         <v>44302</v>
       </c>
-      <c r="B23" s="12" t="str">
+      <c r="B24" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(金)</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C24" s="6">
         <f t="shared" si="0"/>
         <v>69687</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D24" s="6">
         <v>29696</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E24" s="6">
         <v>39991</v>
       </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A24" s="13">
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A25" s="13">
         <v>44301</v>
       </c>
-      <c r="B24" s="12" t="str">
+      <c r="B25" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(木)</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C25" s="6">
         <f t="shared" si="0"/>
         <v>52620</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D25" s="6">
         <v>16637</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E25" s="6">
         <v>35983</v>
       </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A25" s="13">
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A26" s="13">
         <v>44300</v>
       </c>
-      <c r="B25" s="12" t="str">
+      <c r="B26" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(水)</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C26" s="6">
         <f t="shared" si="0"/>
         <v>50996</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D26" s="6">
         <v>9569</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E26" s="6">
         <v>41427</v>
-      </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A26" s="10">
-        <v>44299</v>
-      </c>
-      <c r="B26" s="12" t="str">
-        <f t="shared" ref="B26:B27" si="2">"("&amp;TEXT(A26,"aaa")&amp;")"</f>
-        <v>(火)</v>
-      </c>
-      <c r="C26" s="6">
-        <f t="shared" ref="C26:C27" si="3">SUM(D26:E26)</f>
-        <v>53986</v>
-      </c>
-      <c r="D26" s="6">
-        <v>13896</v>
-      </c>
-      <c r="E26" s="6">
-        <v>40090</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" s="10">
+        <v>44299</v>
+      </c>
+      <c r="B27" s="12" t="str">
+        <f t="shared" ref="B27:B28" si="2">"("&amp;TEXT(A27,"aaa")&amp;")"</f>
+        <v>(火)</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" ref="C27:C28" si="3">SUM(D27:E27)</f>
+        <v>53986</v>
+      </c>
+      <c r="D27" s="6">
+        <v>13896</v>
+      </c>
+      <c r="E27" s="6">
+        <v>40090</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A28" s="10">
         <v>44298</v>
       </c>
-      <c r="B27" s="12" t="str">
+      <c r="B28" s="12" t="str">
         <f t="shared" si="2"/>
         <v>(月)</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C28" s="6">
         <f t="shared" si="3"/>
         <v>96936</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D28" s="6">
         <v>26850</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E28" s="6">
         <v>70086</v>
       </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A28" s="8"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="7"/>
       <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="8"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A30" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="5"/>
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
         <v>6</v>
       </c>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A32" s="1" t="s">
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
         <v>3</v>
       </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F34" s="5"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A36" s="1"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F35" s="5"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A37" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
Flat: latest data (2021-05-21T07:11:35.517Z) {   "date": "2021-05-21T07:11:35.517Z",   "files": [     {       "name": "IRYO-vaccination_data.csv",       "deltaBytes": 50,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data.xlsx"     },     {       "name": "IRYO-vaccination_data.xlsx",       "deltaBytes": 56,       "source": "https://www.kantei.go.jp/jp/content/IRYO-vaccination_data.xlsx"     }   ] }
</commit_message>
<xml_diff>
--- a/IRYO-vaccination_data.xlsx
+++ b/IRYO-vaccination_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t> 内１回目</t>
   </si>
@@ -254,7 +254,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>（5月19日時点）</t>
+    <t>（5月20日時点）</t>
     <rPh sb="2" eb="3">
       <t>ゲツ</t>
     </rPh>
@@ -699,7 +699,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -747,557 +747,577 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="6">
-        <f t="shared" ref="C4:C26" si="0">SUM(D4:E4)</f>
-        <v>5998833</v>
+        <f t="shared" ref="C4:C27" si="0">SUM(D4:E4)</f>
+        <v>6189366</v>
       </c>
       <c r="D4" s="6">
-        <v>3784071</v>
+        <v>3865493</v>
       </c>
       <c r="E4" s="6">
-        <v>2214762</v>
+        <v>2323873</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="13">
-        <v>44335</v>
+        <v>44336</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
-        <v>267866</v>
+        <v>190533</v>
       </c>
       <c r="D5" s="6">
-        <v>88163</v>
+        <v>81422</v>
       </c>
       <c r="E5" s="6">
-        <v>179703</v>
+        <v>109111</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="13">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
-        <v>250244</v>
+        <v>267866</v>
       </c>
       <c r="D6" s="6">
-        <v>94577</v>
+        <v>88163</v>
       </c>
       <c r="E6" s="6">
-        <v>155667</v>
+        <v>179703</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="13">
-        <v>44333</v>
+        <v>44334</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
-        <v>349566</v>
+        <v>250244</v>
       </c>
       <c r="D7" s="6">
-        <v>133843</v>
+        <v>94577</v>
       </c>
       <c r="E7" s="6">
-        <v>215723</v>
+        <v>155667</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="13">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
-        <v>242878</v>
+        <v>349566</v>
       </c>
       <c r="D8" s="6">
-        <v>99493</v>
+        <v>133843</v>
       </c>
       <c r="E8" s="6">
-        <v>143385</v>
+        <v>215723</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="13">
-        <v>44329</v>
+        <v>44330</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
-        <v>219139</v>
+        <v>242878</v>
       </c>
       <c r="D9" s="6">
-        <v>93429</v>
+        <v>99493</v>
       </c>
       <c r="E9" s="6">
-        <v>125710</v>
+        <v>143385</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="13">
-        <v>44328</v>
+        <v>44329</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
-        <v>181720</v>
+        <v>219139</v>
       </c>
       <c r="D10" s="6">
-        <v>82959</v>
+        <v>93429</v>
       </c>
       <c r="E10" s="6">
-        <v>98761</v>
+        <v>125710</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="13">
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>168738</v>
+        <v>181720</v>
       </c>
       <c r="D11" s="6">
-        <v>90287</v>
+        <v>82959</v>
       </c>
       <c r="E11" s="6">
-        <v>78451</v>
+        <v>98761</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="13">
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
-        <v>223504</v>
+        <v>168738</v>
       </c>
       <c r="D12" s="6">
-        <v>155255</v>
+        <v>90287</v>
       </c>
       <c r="E12" s="6">
-        <v>68249</v>
+        <v>78451</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="13">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" si="0"/>
-        <v>140344</v>
+        <v>223504</v>
       </c>
       <c r="D13" s="6">
-        <v>97165</v>
+        <v>155255</v>
       </c>
       <c r="E13" s="6">
-        <v>43179</v>
+        <v>68249</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="13">
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="6">
         <f t="shared" si="0"/>
-        <v>331914</v>
+        <v>140344</v>
       </c>
       <c r="D14" s="6">
-        <v>268978</v>
+        <v>97165</v>
       </c>
       <c r="E14" s="6">
-        <v>62936</v>
+        <v>43179</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="13">
-        <v>44316</v>
+        <v>44322</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C15" s="6">
         <f t="shared" si="0"/>
-        <v>274907</v>
+        <v>331914</v>
       </c>
       <c r="D15" s="6">
-        <v>227667</v>
+        <v>268978</v>
       </c>
       <c r="E15" s="6">
-        <v>47240</v>
+        <v>62936</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="13">
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16" s="6">
         <f t="shared" si="0"/>
-        <v>238273</v>
+        <v>274907</v>
       </c>
       <c r="D16" s="6">
-        <v>194005</v>
+        <v>227667</v>
       </c>
       <c r="E16" s="6">
-        <v>44268</v>
+        <v>47240</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="13">
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" s="6">
         <f t="shared" si="0"/>
-        <v>203174</v>
+        <v>238273</v>
       </c>
       <c r="D17" s="6">
-        <v>172069</v>
+        <v>194005</v>
       </c>
       <c r="E17" s="6">
-        <v>31105</v>
+        <v>44268</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="13">
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18" s="6">
         <f t="shared" si="0"/>
-        <v>263328</v>
+        <v>203174</v>
       </c>
       <c r="D18" s="6">
-        <v>221677</v>
+        <v>172069</v>
       </c>
       <c r="E18" s="6">
-        <v>41651</v>
+        <v>31105</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="13">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" s="6">
         <f t="shared" si="0"/>
-        <v>177672</v>
+        <v>263328</v>
       </c>
       <c r="D19" s="6">
-        <v>147989</v>
+        <v>221677</v>
       </c>
       <c r="E19" s="6">
-        <v>29683</v>
+        <v>41651</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="13">
-        <v>44308</v>
+        <v>44309</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C20" s="6">
         <f t="shared" si="0"/>
-        <v>150489</v>
+        <v>177672</v>
       </c>
       <c r="D20" s="6">
-        <v>128634</v>
+        <v>147989</v>
       </c>
       <c r="E20" s="6">
-        <v>21855</v>
+        <v>29683</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="13">
-        <v>44307</v>
+        <v>44308</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C21" s="6">
         <f t="shared" si="0"/>
-        <v>152884</v>
+        <v>150489</v>
       </c>
       <c r="D21" s="6">
-        <v>126188</v>
+        <v>128634</v>
       </c>
       <c r="E21" s="6">
-        <v>26696</v>
+        <v>21855</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="13">
-        <v>44306</v>
+        <v>44307</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C22" s="6">
         <f t="shared" si="0"/>
-        <v>126419</v>
+        <v>152884</v>
       </c>
       <c r="D22" s="6">
-        <v>98622</v>
+        <v>126188</v>
       </c>
       <c r="E22" s="6">
-        <v>27797</v>
+        <v>26696</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A23" s="15">
-        <v>44305</v>
-      </c>
-      <c r="B23" s="12" t="str">
-        <f t="shared" ref="B23:B26" si="1">"("&amp;TEXT(A23,"aaa")&amp;")"</f>
-        <v>(月)</v>
+      <c r="A23" s="13">
+        <v>44306</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C23" s="6">
         <f t="shared" si="0"/>
-        <v>119032</v>
+        <v>126419</v>
       </c>
       <c r="D23" s="6">
-        <v>64725</v>
+        <v>98622</v>
       </c>
       <c r="E23" s="6">
-        <v>54307</v>
+        <v>27797</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A24" s="13">
+      <c r="A24" s="15">
+        <v>44305</v>
+      </c>
+      <c r="B24" s="12" t="str">
+        <f t="shared" ref="B24:B27" si="1">"("&amp;TEXT(A24,"aaa")&amp;")"</f>
+        <v>(月)</v>
+      </c>
+      <c r="C24" s="6">
+        <f t="shared" si="0"/>
+        <v>119032</v>
+      </c>
+      <c r="D24" s="6">
+        <v>64725</v>
+      </c>
+      <c r="E24" s="6">
+        <v>54307</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A25" s="13">
         <v>44302</v>
       </c>
-      <c r="B24" s="12" t="str">
+      <c r="B25" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(金)</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C25" s="6">
         <f t="shared" si="0"/>
         <v>69687</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D25" s="6">
         <v>29696</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E25" s="6">
         <v>39991</v>
       </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A25" s="13">
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A26" s="13">
         <v>44301</v>
       </c>
-      <c r="B25" s="12" t="str">
+      <c r="B26" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(木)</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C26" s="6">
         <f t="shared" si="0"/>
         <v>52620</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D26" s="6">
         <v>16637</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E26" s="6">
         <v>35983</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A26" s="13">
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A27" s="13">
         <v>44300</v>
       </c>
-      <c r="B26" s="12" t="str">
+      <c r="B27" s="12" t="str">
         <f t="shared" si="1"/>
         <v>(水)</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C27" s="6">
         <f t="shared" si="0"/>
         <v>50996</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D27" s="6">
         <v>9569</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E27" s="6">
         <v>41427</v>
-      </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A27" s="10">
-        <v>44299</v>
-      </c>
-      <c r="B27" s="12" t="str">
-        <f t="shared" ref="B27:B28" si="2">"("&amp;TEXT(A27,"aaa")&amp;")"</f>
-        <v>(火)</v>
-      </c>
-      <c r="C27" s="6">
-        <f t="shared" ref="C27:C28" si="3">SUM(D27:E27)</f>
-        <v>53986</v>
-      </c>
-      <c r="D27" s="6">
-        <v>13896</v>
-      </c>
-      <c r="E27" s="6">
-        <v>40090</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" s="10">
+        <v>44299</v>
+      </c>
+      <c r="B28" s="12" t="str">
+        <f t="shared" ref="B28:B29" si="2">"("&amp;TEXT(A28,"aaa")&amp;")"</f>
+        <v>(火)</v>
+      </c>
+      <c r="C28" s="6">
+        <f t="shared" ref="C28:C29" si="3">SUM(D28:E28)</f>
+        <v>53986</v>
+      </c>
+      <c r="D28" s="6">
+        <v>13896</v>
+      </c>
+      <c r="E28" s="6">
+        <v>40090</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A29" s="10">
         <v>44298</v>
       </c>
-      <c r="B28" s="12" t="str">
+      <c r="B29" s="12" t="str">
         <f t="shared" si="2"/>
         <v>(月)</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C29" s="6">
         <f t="shared" si="3"/>
         <v>96936</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D29" s="6">
         <v>26850</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E29" s="6">
         <v>70086</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A29" s="8"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="7"/>
       <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A31" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="5"/>
       <c r="F31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
         <v>6</v>
       </c>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A33" s="1" t="s">
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="7"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
         <v>3</v>
       </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="F35" s="5"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A37" s="1"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F36" s="5"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A38" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>